<commit_message>
[ENH] pabi_account_report, new SQL
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t xml:space="preserve">Asset Register Report</t>
   </si>
@@ -40,40 +40,40 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Asset Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsible Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsible Person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Category</t>
   </si>
   <si>
     <t xml:space="preserve">Account Name</t>
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:BB19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,28 +429,23 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="8"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
@@ -461,7 +456,7 @@
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
@@ -472,16 +467,18 @@
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="1"/>
@@ -489,7 +486,7 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="1"/>
@@ -497,7 +494,7 @@
     </row>
     <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="1"/>
@@ -505,7 +502,7 @@
     </row>
     <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -513,7 +510,7 @@
     </row>
     <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
@@ -521,7 +518,7 @@
     </row>
     <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="1"/>
@@ -529,7 +526,7 @@
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="1"/>
@@ -537,7 +534,7 @@
     </row>
     <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="1"/>
@@ -545,7 +542,7 @@
     </row>
     <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="1"/>
@@ -553,7 +550,7 @@
     </row>
     <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="1"/>
@@ -568,10 +565,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>18</v>
@@ -583,7 +580,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>21</v>
@@ -637,13 +634,13 @@
         <v>37</v>
       </c>
       <c r="Y19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Z19" s="10" t="s">
+      <c r="AA19" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="AA19" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="AB19" s="10" t="s">
         <v>38</v>
@@ -721,7 +718,7 @@
         <v>61</v>
       </c>
       <c r="BA19" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BB19" s="10" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
[FIX] #2661 asset_register query wrong
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -118,10 +118,10 @@
     <t xml:space="preserve">Owner Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost Cetner Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Cetner Name</t>
+    <t xml:space="preserve">Cost Center Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Center Name</t>
   </si>
   <si>
     <t xml:space="preserve">Source of Fund</t>
@@ -373,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:BB19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T20" activeCellId="0" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[FIX] #2701 Asset register report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t xml:space="preserve">Asset Register Report</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">To</t>
   </si>
   <si>
-    <t xml:space="preserve">Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
     <t xml:space="preserve">Asset Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Account Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Responsible Person</t>
   </si>
   <si>
@@ -58,9 +58,30 @@
     <t xml:space="preserve">Room</t>
   </si>
   <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asset Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Source of Budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsector</t>
+  </si>
+  <si>
     <t xml:space="preserve">Current Year</t>
   </si>
   <si>
@@ -73,9 +94,6 @@
     <t xml:space="preserve">Product Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Account Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account Name</t>
   </si>
   <si>
@@ -131,15 +149,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fund of Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector</t>
   </si>
   <si>
     <t xml:space="preserve">Responsible Person ID</t>
@@ -377,10 +386,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BD19"/>
+  <dimension ref="A1:BD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,12 +484,9 @@
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
@@ -558,182 +564,238 @@
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" s="11" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" s="11" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="T26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V26" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="Y26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="U19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="V19" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="W19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="X19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y19" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA19" s="10" t="s">
+      <c r="AA26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AB19" s="10" t="s">
+      <c r="AB26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC19" s="10" t="s">
+      <c r="AC26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AD19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG19" s="10" t="s">
+      <c r="AD26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AH19" s="10" t="s">
+      <c r="AE26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AI19" s="10" t="s">
+      <c r="AF26" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AJ19" s="10" t="s">
+      <c r="AG26" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="AK19" s="10" t="s">
+      <c r="AH26" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AL19" s="10" t="s">
+      <c r="AI26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="AM19" s="10" t="s">
+      <c r="AJ26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AN19" s="10" t="s">
+      <c r="AK26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AO19" s="10" t="s">
+      <c r="AL26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AP19" s="10" t="s">
+      <c r="AM26" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AQ19" s="10" t="s">
+      <c r="AN26" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AR19" s="10" t="s">
+      <c r="AO26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AS19" s="10" t="s">
+      <c r="AP26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AT19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AV19" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AW19" s="10" t="s">
+      <c r="AT26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AX19" s="10" t="s">
+      <c r="AU26" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AY19" s="10" t="s">
+      <c r="AV26" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AZ19" s="10" t="s">
+      <c r="AW26" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="BA19" s="10" t="s">
+      <c r="AX26" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="BB19" s="10" t="s">
+      <c r="AY26" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="BC19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="BD19" s="10" t="s">
+      <c r="AZ26" s="10" t="s">
         <v>64</v>
+      </c>
+      <c r="BA26" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="BB26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD26" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] add sheet group by in asset_register
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Asset Register Report" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Accum. Depre. Group By GL" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t xml:space="preserve">Asset Register Report</t>
   </si>
@@ -232,9 +233,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -320,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,6 +370,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -389,7 +404,7 @@
   <dimension ref="A1:BD26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,4 +822,59 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="12" width="16.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX] asset register report order_by code
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -393,6 +393,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -869,6 +881,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:H1048576">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$A1="Total"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
#4037-AssetRegisterReport Module: pabi_account_report https://mobileapp.nstda.or.th/redmine/issues/4037 เปลี่ยนชื่อ Org ใน excel เป็น Org Owner ช่อง Org Owner ดึงจาก owner_code
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_asset_register.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Asset Register Report</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Asset State</t>
+  </si>
+  <si>
+    <t>Org Owner</t>
   </si>
 </sst>
 </file>
@@ -338,6 +341,14 @@
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -356,19 +367,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -647,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BJ21" sqref="BJ21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -891,7 +894,7 @@
     </row>
     <row r="26" spans="1:57" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>23</v>
@@ -1113,7 +1116,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A1="Total"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>